<commit_message>
Restored database Models/Final Raiting.Context.cs Added Controllers/Table22Controller.cs Added empty Controllers
</commit_message>
<xml_diff>
--- a/RatingUniversity/Files/22_osnashennost_laboratoriy.xlsx
+++ b/RatingUniversity/Files/22_osnashennost_laboratoriy.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilechka\Desktop\last scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repositories\Raiting\RatingUniversity\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">М А Ъ Л У М О Т </t>
   </si>
@@ -82,11 +82,14 @@
   <si>
     <t xml:space="preserve">** бир неча фанлар учун фойдаланиладиган лаборатория ёки ёрдамчи асбоб-ускуналар бўйича маълумотлар умумий берилади. </t>
   </si>
+  <si>
+    <t>Жадвал 22</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -221,6 +224,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -519,6 +525,11 @@
     <col min="7" max="16384" width="25.85546875" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>

</xml_diff>